<commit_message>
Basic and meal item test w/ pages update
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,27 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajovic\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6F8ED8-9574-409A-BADD-C318F7645284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Meals" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="Meal Search Results" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Meals" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>LOCATION</t>
   </si>
@@ -35,6 +26,9 @@
     <t>Arbor Hill - Albany</t>
   </si>
   <si>
+    <t>http://demo.yo-meals.com/meals&amp;type=veg--non-veg&amp;mealtype=breakfast--brunch--lunch&amp;price=40-574</t>
+  </si>
+  <si>
     <t>Baked Caldereta</t>
   </si>
   <si>
@@ -47,6 +41,9 @@
     <t>Palak Paneer</t>
   </si>
   <si>
+    <t>http://demo.yo-meals.com/meals&amp;cuisine=italian--mexican&amp;keywords=chicken&amp;order=low</t>
+  </si>
+  <si>
     <t>Chicken Strips Wings</t>
   </si>
   <si>
@@ -56,12 +53,21 @@
     <t>New Scotland - Albany</t>
   </si>
   <si>
+    <t>http://demo.yo-meals.com/meals&amp;mealtype=brunch&amp;cuisine=italian&amp;price=12-18&amp;order=low&amp;chef=1</t>
+  </si>
+  <si>
     <t>Library Road - Albany</t>
   </si>
   <si>
+    <t>http://demo.yo-meals.com/meals</t>
+  </si>
+  <si>
     <t>Manning Boulevard - Albany</t>
   </si>
   <si>
+    <t>http://demo.yo-meals.com/meals&amp;type=veg&amp;mealtype=dinner&amp;cuisine=american--british--caribbean--chinese--french--japanese--mediterranean&amp;price=90-700&amp;order=high</t>
+  </si>
+  <si>
     <t>T-bone Huevos Steak</t>
   </si>
   <si>
@@ -123,48 +129,32 @@
   </si>
   <si>
     <t>http://demo.yo-meals.com/meal/cashew-meatloaf-chicken</t>
-  </si>
-  <si>
-    <t>http://demo.yo-meals.com/meal/linguica-southwestern-benedict</t>
-  </si>
-  <si>
-    <t>http://demo.yo-meals.com/meal/chocolate-chip-scrambler-pancakes</t>
-  </si>
-  <si>
-    <t>http://demo.yo-meals.com/meal/buffalo-wings-shrimp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -172,7 +162,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -182,46 +172,51 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -411,32 +406,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="122.77734375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="26.86"/>
+    <col customWidth="1" min="2" max="2" width="25.86"/>
+    <col customWidth="1" min="3" max="3" width="22.29"/>
+    <col customWidth="1" min="4" max="4" width="19.43"/>
+    <col customWidth="1" min="5" max="5" width="18.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,264 +437,271 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="T7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="3">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="B22" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B7"/>
+  </hyperlinks>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="56.29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>